<commit_message>
Now creates folders, and starting to add training to the BayesingNetwork
</commit_message>
<xml_diff>
--- a/ClassDia.xlsx
+++ b/ClassDia.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Menu</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>BayesingNetwork</t>
+  </si>
+  <si>
+    <t>string _lemmatizingWords</t>
+  </si>
+  <si>
+    <t>pub Dictionary&lt;s,i&gt; WordAndcount(void)</t>
+  </si>
+  <si>
+    <t>FileObj[] getTestData()</t>
+  </si>
+  <si>
+    <t>FileObj[] GetSavedBayesingNetworks()</t>
+  </si>
+  <si>
+    <t>Train()</t>
   </si>
 </sst>
 </file>
@@ -395,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:F16"/>
+  <dimension ref="B5:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,35 +444,48 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -469,6 +497,16 @@
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated classdia, starting to get the AI trianing to work :)
</commit_message>
<xml_diff>
--- a/ClassDia.xlsx
+++ b/ClassDia.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Subjects\3Year\Interactive Artificial Intelligence\AutoMaticTextClassification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Subjects\3Year\Interactive Artificial Intelligence\AutoMaticTextClassification\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DFD24-ECD1-4D20-83F8-DD3A89F1C793}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,20 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Menu</t>
   </si>
   <si>
-    <t>StartUp(void)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Catagory </t>
   </si>
   <si>
-    <t>Result(string mostViable, double percent)</t>
-  </si>
-  <si>
     <t>Pub AddText(string text)</t>
   </si>
   <si>
@@ -53,9 +48,6 @@
     <t>List&lt;Catagory&gt;  _knownInfromation</t>
   </si>
   <si>
-    <t>string _currentText</t>
-  </si>
-  <si>
     <t>Pub GetTotalWods(void) : count</t>
   </si>
   <si>
@@ -77,19 +69,52 @@
     <t>pub Dictionary&lt;s,i&gt; WordAndcount(void)</t>
   </si>
   <si>
-    <t>FileObj[] getTestData()</t>
-  </si>
-  <si>
-    <t>FileObj[] GetSavedBayesingNetworks()</t>
-  </si>
-  <si>
-    <t>Train()</t>
+    <t>string _TrainingDataFolder</t>
+  </si>
+  <si>
+    <t>string _analisingText</t>
+  </si>
+  <si>
+    <t>BayesingNetwork _bn</t>
+  </si>
+  <si>
+    <t>FileObj</t>
+  </si>
+  <si>
+    <t>pub StartUp(void)</t>
+  </si>
+  <si>
+    <t>pub Result(string mostViable, double percent)</t>
+  </si>
+  <si>
+    <t>pub SaveBayesingNetwork()</t>
+  </si>
+  <si>
+    <t>pub Train()</t>
+  </si>
+  <si>
+    <t>pub FileObj[] getTestData()</t>
+  </si>
+  <si>
+    <t>pub FileObj[] GetSavedBayesingNetworks()</t>
+  </si>
+  <si>
+    <t>pub FileObj[] GetTrainingData()</t>
+  </si>
+  <si>
+    <t>pub string[] GetLemmatizingWords()</t>
+  </si>
+  <si>
+    <t>pub bool SaveBayesingToFile(string folderName, List&lt;CategoryObj&gt; bayesingNetwork)</t>
+  </si>
+  <si>
+    <t>pub BayesingNetwork[] GetSavedBayesingNetworks()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,104 +434,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>18</v>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>